<commit_message>
Updated Burndown Chart for 07., 08., 09. February.
</commit_message>
<xml_diff>
--- a/Documentation/Burndown_Chart.xlsx
+++ b/Documentation/Burndown_Chart.xlsx
@@ -1709,7 +1709,7 @@
   <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1796,8 +1796,12 @@
       <c r="C2" s="5">
         <v>0</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -1915,87 +1919,87 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" ref="C4:W4" si="1">$B$3/COUNTA($C$1:$W$1)</f>
         <v>3.3809523809523809</v>
       </c>
       <c r="D4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="E4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="F4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="G4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="H4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="I4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="J4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="K4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="L4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="M4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="N4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="O4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="P4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="Q4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="R4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="S4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="T4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="U4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="V4" s="8">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
       <c r="W4" s="9">
-        <f>$B$3/COUNTA($C$1:$W$1)</f>
+        <f t="shared" si="1"/>
         <v>3.3809523809523809</v>
       </c>
     </row>
@@ -2013,79 +2017,79 @@
         <v>64.238095238095241</v>
       </c>
       <c r="E5" s="11">
-        <f t="shared" ref="E5:W5" si="1">D5-E4</f>
+        <f t="shared" ref="E5:W5" si="2">D5-E4</f>
         <v>60.857142857142861</v>
       </c>
       <c r="F5" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>57.476190476190482</v>
       </c>
       <c r="G5" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>54.095238095238102</v>
       </c>
       <c r="H5" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50.714285714285722</v>
       </c>
       <c r="I5" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47.333333333333343</v>
       </c>
       <c r="J5" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43.952380952380963</v>
       </c>
       <c r="K5" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40.571428571428584</v>
       </c>
       <c r="L5" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37.190476190476204</v>
       </c>
       <c r="M5" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33.809523809523824</v>
       </c>
       <c r="N5" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30.428571428571445</v>
       </c>
       <c r="O5" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27.047619047619065</v>
       </c>
       <c r="P5" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23.666666666666686</v>
       </c>
       <c r="Q5" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20.285714285714306</v>
       </c>
       <c r="R5" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16.904761904761926</v>
       </c>
       <c r="S5" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.523809523809545</v>
       </c>
       <c r="T5" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10.142857142857164</v>
       </c>
       <c r="U5" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.7619047619047823</v>
       </c>
       <c r="V5" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.3809523809524014</v>
       </c>
       <c r="W5" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.042810365310288E-14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Burndown Chart updated for until today (12/02/17).
</commit_message>
<xml_diff>
--- a/Documentation/Burndown_Chart.xlsx
+++ b/Documentation/Burndown_Chart.xlsx
@@ -1709,7 +1709,7 @@
   <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,9 +1802,15 @@
       <c r="E2" s="5">
         <v>0</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>

</xml_diff>

<commit_message>
Burn down chart backwards-adjusted, in reaction to a miscommunication between Philip and the Scrum Master (Konstantin).
</commit_message>
<xml_diff>
--- a/Documentation/Burndown_Chart.xlsx
+++ b/Documentation/Burndown_Chart.xlsx
@@ -346,61 +346,61 @@
                   <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>71</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>71</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>71</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>71</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>71</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>71</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>71</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>71</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>71</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>71</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>71</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>71</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>71</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>71</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>71</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>71</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>71</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>71</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1709,7 +1709,7 @@
   <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1800,13 +1800,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="5">
         <v>0</v>
       </c>
       <c r="G2" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" s="5">
         <v>0</v>
@@ -1844,79 +1844,79 @@
       </c>
       <c r="E3" s="7">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F3" s="7">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G3" s="7">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H3" s="7">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I3" s="7">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J3" s="7">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K3" s="7">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L3" s="7">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M3" s="7">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N3" s="7">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="O3" s="7">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P3" s="7">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Q3" s="7">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="R3" s="7">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="S3" s="7">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="T3" s="7">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="U3" s="7">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="V3" s="7">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W3" s="2">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Increased the start value of this sprint to 77 (from 71, +6) in result of the addition of three new (0-2) tasks created. See today's protocol for reference.
</commit_message>
<xml_diff>
--- a/Documentation/Burndown_Chart.xlsx
+++ b/Documentation/Burndown_Chart.xlsx
@@ -340,67 +340,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>71</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>71</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>69</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>69</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>69</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>69</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>69</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>69</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>69</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>69</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>69</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>69</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>69</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>69</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>69</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>69</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>69</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>69</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -437,67 +437,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>67.61904761904762</c:v>
+                  <c:v>73.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64.238095238095241</c:v>
+                  <c:v>69.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60.857142857142861</c:v>
+                  <c:v>65.999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57.476190476190482</c:v>
+                  <c:v>62.333333333333321</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54.095238095238102</c:v>
+                  <c:v>58.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50.714285714285722</c:v>
+                  <c:v>54.999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>47.333333333333343</c:v>
+                  <c:v>51.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43.952380952380963</c:v>
+                  <c:v>47.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.571428571428584</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37.190476190476204</c:v>
+                  <c:v>40.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33.809523809523824</c:v>
+                  <c:v>36.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30.428571428571445</c:v>
+                  <c:v>33.000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>27.047619047619065</c:v>
+                  <c:v>29.333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>23.666666666666686</c:v>
+                  <c:v>25.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20.285714285714306</c:v>
+                  <c:v>22.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16.904761904761926</c:v>
+                  <c:v>18.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>13.523809523809545</c:v>
+                  <c:v>14.66666666666667</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.142857142857164</c:v>
+                  <c:v>11.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.7619047619047823</c:v>
+                  <c:v>7.3333333333333375</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.3809523809524014</c:v>
+                  <c:v>3.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.042810365310288E-14</c:v>
+                  <c:v>4.4408920985006262E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1709,7 +1709,7 @@
   <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1832,91 +1832,91 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C3" s="7">
         <f>B3-C2</f>
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D3" s="7">
         <f t="shared" ref="D3:W3" si="0">C3-D2</f>
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E3" s="7">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="F3" s="7">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="G3" s="7">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="H3" s="7">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="I3" s="7">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="J3" s="7">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="K3" s="7">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="L3" s="7">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="M3" s="7">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="N3" s="7">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="O3" s="7">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="P3" s="7">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="Q3" s="7">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="R3" s="7">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="S3" s="7">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="T3" s="7">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="U3" s="7">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="V3" s="7">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="W3" s="2">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -1926,87 +1926,87 @@
       <c r="B4" s="2"/>
       <c r="C4" s="8">
         <f t="shared" ref="C4:W4" si="1">$B$3/COUNTA($C$1:$W$1)</f>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="D4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="E4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="F4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="G4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="H4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="I4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="J4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="K4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="L4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="M4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="N4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="O4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="P4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="Q4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="R4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="S4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="T4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="U4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="V4" s="8">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="W4" s="9">
         <f t="shared" si="1"/>
-        <v>3.3809523809523809</v>
+        <v>3.6666666666666665</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -2016,87 +2016,87 @@
       <c r="B5" s="10"/>
       <c r="C5" s="11">
         <f>$B$3-C4</f>
-        <v>67.61904761904762</v>
+        <v>73.333333333333329</v>
       </c>
       <c r="D5" s="11">
         <f>C5-D4</f>
-        <v>64.238095238095241</v>
+        <v>69.666666666666657</v>
       </c>
       <c r="E5" s="11">
         <f t="shared" ref="E5:W5" si="2">D5-E4</f>
-        <v>60.857142857142861</v>
+        <v>65.999999999999986</v>
       </c>
       <c r="F5" s="11">
         <f t="shared" si="2"/>
-        <v>57.476190476190482</v>
+        <v>62.333333333333321</v>
       </c>
       <c r="G5" s="11">
         <f t="shared" si="2"/>
-        <v>54.095238095238102</v>
+        <v>58.666666666666657</v>
       </c>
       <c r="H5" s="11">
         <f t="shared" si="2"/>
-        <v>50.714285714285722</v>
+        <v>54.999999999999993</v>
       </c>
       <c r="I5" s="11">
         <f t="shared" si="2"/>
-        <v>47.333333333333343</v>
+        <v>51.333333333333329</v>
       </c>
       <c r="J5" s="11">
         <f t="shared" si="2"/>
-        <v>43.952380952380963</v>
+        <v>47.666666666666664</v>
       </c>
       <c r="K5" s="11">
         <f t="shared" si="2"/>
-        <v>40.571428571428584</v>
+        <v>44</v>
       </c>
       <c r="L5" s="11">
         <f t="shared" si="2"/>
-        <v>37.190476190476204</v>
+        <v>40.333333333333336</v>
       </c>
       <c r="M5" s="11">
         <f t="shared" si="2"/>
-        <v>33.809523809523824</v>
+        <v>36.666666666666671</v>
       </c>
       <c r="N5" s="11">
         <f t="shared" si="2"/>
-        <v>30.428571428571445</v>
+        <v>33.000000000000007</v>
       </c>
       <c r="O5" s="11">
         <f t="shared" si="2"/>
-        <v>27.047619047619065</v>
+        <v>29.333333333333339</v>
       </c>
       <c r="P5" s="11">
         <f t="shared" si="2"/>
-        <v>23.666666666666686</v>
+        <v>25.666666666666671</v>
       </c>
       <c r="Q5" s="11">
         <f t="shared" si="2"/>
-        <v>20.285714285714306</v>
+        <v>22.000000000000004</v>
       </c>
       <c r="R5" s="11">
         <f t="shared" si="2"/>
-        <v>16.904761904761926</v>
+        <v>18.333333333333336</v>
       </c>
       <c r="S5" s="11">
         <f t="shared" si="2"/>
-        <v>13.523809523809545</v>
+        <v>14.66666666666667</v>
       </c>
       <c r="T5" s="11">
         <f t="shared" si="2"/>
-        <v>10.142857142857164</v>
+        <v>11.000000000000004</v>
       </c>
       <c r="U5" s="11">
         <f t="shared" si="2"/>
-        <v>6.7619047619047823</v>
+        <v>7.3333333333333375</v>
       </c>
       <c r="V5" s="11">
         <f t="shared" si="2"/>
-        <v>3.3809523809524014</v>
+        <v>3.666666666666671</v>
       </c>
       <c r="W5" s="12">
         <f t="shared" si="2"/>
-        <v>2.042810365310288E-14</v>
+        <v>4.4408920985006262E-15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Burndown chart updated as result of the daily scrum meeting today.
</commit_message>
<xml_diff>
--- a/Documentation/Burndown_Chart.xlsx
+++ b/Documentation/Burndown_Chart.xlsx
@@ -193,9 +193,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="166" formatCode="#,##0\ _€"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="#,##0.0"/>
+    <numFmt numFmtId="164" formatCode="#,##0\ _€"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -513,10 +513,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -564,13 +564,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -720,37 +720,37 @@
                   <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>74.5</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>74.5</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>74.5</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>74.5</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>74.5</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>74.5</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>74.5</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>74.5</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>74.5</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>74.5</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>74.5</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1863,7 +1863,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.5</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1879,7 +1879,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -5399,7 +5398,7 @@
   <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5497,7 +5496,9 @@
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
       <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
+      <c r="M2" s="23">
+        <v>1</v>
+      </c>
       <c r="N2" s="23"/>
       <c r="O2" s="23"/>
       <c r="P2" s="23"/>
@@ -5639,7 +5640,7 @@
       </c>
       <c r="M6" s="37">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="37">
         <f t="shared" si="0"/>
@@ -5731,47 +5732,47 @@
       </c>
       <c r="M7" s="7">
         <f t="shared" si="1"/>
-        <v>74.5</v>
+        <v>73.5</v>
       </c>
       <c r="N7" s="7">
         <f t="shared" si="1"/>
-        <v>74.5</v>
+        <v>73.5</v>
       </c>
       <c r="O7" s="7">
         <f t="shared" si="1"/>
-        <v>74.5</v>
+        <v>73.5</v>
       </c>
       <c r="P7" s="7">
         <f t="shared" si="1"/>
-        <v>74.5</v>
+        <v>73.5</v>
       </c>
       <c r="Q7" s="7">
         <f t="shared" si="1"/>
-        <v>74.5</v>
+        <v>73.5</v>
       </c>
       <c r="R7" s="7">
         <f t="shared" si="1"/>
-        <v>74.5</v>
+        <v>73.5</v>
       </c>
       <c r="S7" s="7">
         <f t="shared" si="1"/>
-        <v>74.5</v>
+        <v>73.5</v>
       </c>
       <c r="T7" s="7">
         <f t="shared" si="1"/>
-        <v>74.5</v>
+        <v>73.5</v>
       </c>
       <c r="U7" s="7">
         <f t="shared" si="1"/>
-        <v>74.5</v>
+        <v>73.5</v>
       </c>
       <c r="V7" s="7">
         <f t="shared" si="1"/>
-        <v>74.5</v>
+        <v>73.5</v>
       </c>
       <c r="W7" s="2">
         <f t="shared" si="1"/>
-        <v>74.5</v>
+        <v>73.5</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -6551,7 +6552,7 @@
       </c>
       <c r="B2" s="33">
         <f>Sprint_One!B7-Sprint_One!W7</f>
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated burndown chart in effect of the daily scrum meeting today
</commit_message>
<xml_diff>
--- a/Documentation/Burndown_Chart.xlsx
+++ b/Documentation/Burndown_Chart.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Southampton\solent\Software Systems Development\Scrum\Github\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3schak76\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11310" tabRatio="587"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="587"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint_One" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Velocity_Chart" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint_One (Deprecated)" sheetId="1" state="hidden" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -191,7 +191,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0\ _€"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -461,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -573,9 +573,33 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -591,9 +615,1579 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Burndown-Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Actual</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint_One!$C$7:$W$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>71.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>71.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>71.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>71.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>70.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6563-483E-A12C-864B2E4FE692}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ideal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint_One!$C$9:$W$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>71.428571428571431</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67.857142857142861</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.285714285714292</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60.714285714285722</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57.142857142857153</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53.571428571428584</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50.000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46.428571428571445</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42.857142857142875</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39.285714285714306</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>35.714285714285737</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32.142857142857167</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28.571428571428594</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25.000000000000021</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21.428571428571448</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17.857142857142875</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14.285714285714304</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10.714285714285733</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.1428571428571619</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.5714285714285903</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.865174681370263E-14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6563-483E-A12C-864B2E4FE692}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="232847640"/>
+        <c:axId val="232848032"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="232847640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Days in Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="232848032"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="232848032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Remaining</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Effort Hours</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="232847640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Burndown-Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Actual</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint_Two!$C$7:$W$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8A22-4D2A-B82F-502C025A796D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ideal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint_Two!$C$9:$W$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8A22-4D2A-B82F-502C025A796D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="232848816"/>
+        <c:axId val="233795632"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="232848816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Days in Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="233795632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="233795632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Remaining</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Effort Hours</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="232848816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Velocity Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Velocity_Chart!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>one</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>two</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>three</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>four</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Velocity_Chart!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-0ED7-4308-8C5A-9471866D8495}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="233796416"/>
+        <c:axId val="233796808"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="233796416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="233796808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="233796808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Work Done</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="233796416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -685,80 +2279,80 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sprint_One!$C$7:$W$7</c:f>
+              <c:f>'Sprint_One (Deprecated)'!$C$3:$W$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>75</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>75</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>73</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>72.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>72.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>72.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>71.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>71.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>71.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>71.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>71.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>71.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>71.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>71.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>71.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>71.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>71.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6563-483E-A12C-864B2E4FE692}"/>
+              <c16:uniqueId val="{00000000-9251-4BA3-ADAD-D0E9A2AE2542}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -782,80 +2376,80 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sprint_One!$C$9:$W$9</c:f>
+              <c:f>'Sprint_One (Deprecated)'!$C$5:$W$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>71.428571428571431</c:v>
+                  <c:v>73.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>67.857142857142861</c:v>
+                  <c:v>69.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64.285714285714292</c:v>
+                  <c:v>65.999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60.714285714285722</c:v>
+                  <c:v>62.333333333333321</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57.142857142857153</c:v>
+                  <c:v>58.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53.571428571428584</c:v>
+                  <c:v>54.999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50.000000000000014</c:v>
+                  <c:v>51.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>46.428571428571445</c:v>
+                  <c:v>47.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42.857142857142875</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>39.285714285714306</c:v>
+                  <c:v>40.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>35.714285714285737</c:v>
+                  <c:v>36.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32.142857142857167</c:v>
+                  <c:v>33.000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28.571428571428594</c:v>
+                  <c:v>29.333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25.000000000000021</c:v>
+                  <c:v>25.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21.428571428571448</c:v>
+                  <c:v>22.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>17.857142857142875</c:v>
+                  <c:v>18.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14.285714285714304</c:v>
+                  <c:v>14.66666666666667</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.714285714285733</c:v>
+                  <c:v>11.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.1428571428571619</c:v>
+                  <c:v>7.3333333333333375</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.5714285714285903</c:v>
+                  <c:v>3.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.865174681370263E-14</c:v>
+                  <c:v>4.4408920985006262E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6563-483E-A12C-864B2E4FE692}"/>
+              <c16:uniqueId val="{00000001-9251-4BA3-ADAD-D0E9A2AE2542}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -868,11 +2462,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="400622560"/>
-        <c:axId val="400622888"/>
+        <c:axId val="233797592"/>
+        <c:axId val="233797984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="400622560"/>
+        <c:axId val="233797592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -969,7 +2563,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400622888"/>
+        <c:crossAx val="233797984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -977,7 +2571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="400622888"/>
+        <c:axId val="233797984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,1569 +2682,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400622560"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Burndown-Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Actual</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sprint_Two!$C$7:$W$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8A22-4D2A-B82F-502C025A796D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Ideal</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sprint_Two!$C$9:$W$9</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8A22-4D2A-B82F-502C025A796D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="400622560"/>
-        <c:axId val="400622888"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="400622560"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Days in Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="400622888"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="400622888"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Remaining</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Effort Hours</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="400622560"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Velocity Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Velocity_Chart!$A$2:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>one</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>two</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>three</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>four</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Velocity_Chart!$B$2:$B$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-0ED7-4308-8C5A-9471866D8495}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="362434096"/>
-        <c:axId val="362434424"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="362434096"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="362434424"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="362434424"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Work Done</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="362434096"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Burndown-Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Actual</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint_One (Deprecated)'!$C$3:$W$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>74.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9251-4BA3-ADAD-D0E9A2AE2542}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Ideal</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint_One (Deprecated)'!$C$5:$W$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>73.333333333333329</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>69.666666666666657</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>65.999999999999986</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>62.333333333333321</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>58.666666666666657</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>54.999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>51.333333333333329</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>47.666666666666664</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>40.333333333333336</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>36.666666666666671</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>33.000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>29.333333333333339</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>25.666666666666671</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>22.000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>18.333333333333336</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>14.66666666666667</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>11.000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>7.3333333333333375</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.666666666666671</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4.4408920985006262E-15</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9251-4BA3-ADAD-D0E9A2AE2542}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="400622560"/>
-        <c:axId val="400622888"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="400622560"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Days in Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="400622888"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="400622888"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Remaining</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Effort Hours</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="400622560"/>
+        <c:crossAx val="233797592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5398,10 +5430,10 @@
   <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
   </cols>
@@ -5482,23 +5514,591 @@
         <v>6</v>
       </c>
       <c r="B2" s="16"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36">
+        <v>1</v>
+      </c>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36">
+        <v>1</v>
+      </c>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="40"/>
+    </row>
+    <row r="3" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42"/>
+      <c r="S3" s="42"/>
+      <c r="T3" s="42"/>
+      <c r="U3" s="42"/>
+      <c r="V3" s="42"/>
+      <c r="W3" s="43"/>
+    </row>
+    <row r="4" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42">
+        <v>1</v>
+      </c>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="R4" s="42"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="42"/>
+      <c r="V4" s="42"/>
+      <c r="W4" s="43"/>
+    </row>
+    <row r="5" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45">
+        <v>0.5</v>
+      </c>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
+      <c r="T5" s="45"/>
+      <c r="U5" s="45"/>
+      <c r="V5" s="45"/>
+      <c r="W5" s="46"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="37">
+        <f>SUM(C2:C5)</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="37">
+        <f t="shared" ref="D6:W6" si="0">SUM(D2:D5)</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F6" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H6" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="37">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="J6" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N6" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R6" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S6" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U6" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V6" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W6" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="35">
+        <v>75</v>
+      </c>
+      <c r="C7" s="7">
+        <f>B7-C6</f>
+        <v>75</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" ref="D7:W7" si="1">C7-D6</f>
+        <v>75</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="G7" s="7">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="H7" s="7">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="I7" s="7">
+        <f t="shared" si="1"/>
+        <v>72.5</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="1"/>
+        <v>72.5</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="1"/>
+        <v>72.5</v>
+      </c>
+      <c r="L7" s="7">
+        <f t="shared" si="1"/>
+        <v>72.5</v>
+      </c>
+      <c r="M7" s="7">
+        <f t="shared" si="1"/>
+        <v>71.5</v>
+      </c>
+      <c r="N7" s="7">
+        <f t="shared" si="1"/>
+        <v>71.5</v>
+      </c>
+      <c r="O7" s="7">
+        <f t="shared" si="1"/>
+        <v>71.5</v>
+      </c>
+      <c r="P7" s="7">
+        <f t="shared" si="1"/>
+        <v>71.5</v>
+      </c>
+      <c r="Q7" s="7">
+        <f t="shared" si="1"/>
+        <v>70.5</v>
+      </c>
+      <c r="R7" s="7">
+        <f t="shared" si="1"/>
+        <v>70.5</v>
+      </c>
+      <c r="S7" s="7">
+        <f t="shared" si="1"/>
+        <v>70.5</v>
+      </c>
+      <c r="T7" s="7">
+        <f t="shared" si="1"/>
+        <v>70.5</v>
+      </c>
+      <c r="U7" s="7">
+        <f t="shared" si="1"/>
+        <v>70.5</v>
+      </c>
+      <c r="V7" s="7">
+        <f t="shared" si="1"/>
+        <v>70.5</v>
+      </c>
+      <c r="W7" s="2">
+        <f t="shared" si="1"/>
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="8">
+        <f t="shared" ref="C8:W8" si="2">$B$7/COUNTA($C$1:$W$1)</f>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="D8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="G8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="H8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="I8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="J8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="K8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="L8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="M8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="N8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="O8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="P8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="Q8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="R8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="S8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="T8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="U8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="V8" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="W8" s="9">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11">
+        <f>$B$7-C8</f>
+        <v>71.428571428571431</v>
+      </c>
+      <c r="D9" s="11">
+        <f>C9-D8</f>
+        <v>67.857142857142861</v>
+      </c>
+      <c r="E9" s="11">
+        <f t="shared" ref="E9:W9" si="3">D9-E8</f>
+        <v>64.285714285714292</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="3"/>
+        <v>60.714285714285722</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" si="3"/>
+        <v>57.142857142857153</v>
+      </c>
+      <c r="H9" s="11">
+        <f t="shared" si="3"/>
+        <v>53.571428571428584</v>
+      </c>
+      <c r="I9" s="11">
+        <f t="shared" si="3"/>
+        <v>50.000000000000014</v>
+      </c>
+      <c r="J9" s="11">
+        <f t="shared" si="3"/>
+        <v>46.428571428571445</v>
+      </c>
+      <c r="K9" s="11">
+        <f t="shared" si="3"/>
+        <v>42.857142857142875</v>
+      </c>
+      <c r="L9" s="11">
+        <f t="shared" si="3"/>
+        <v>39.285714285714306</v>
+      </c>
+      <c r="M9" s="11">
+        <f t="shared" si="3"/>
+        <v>35.714285714285737</v>
+      </c>
+      <c r="N9" s="11">
+        <f t="shared" si="3"/>
+        <v>32.142857142857167</v>
+      </c>
+      <c r="O9" s="11">
+        <f t="shared" si="3"/>
+        <v>28.571428571428594</v>
+      </c>
+      <c r="P9" s="11">
+        <f t="shared" si="3"/>
+        <v>25.000000000000021</v>
+      </c>
+      <c r="Q9" s="11">
+        <f t="shared" si="3"/>
+        <v>21.428571428571448</v>
+      </c>
+      <c r="R9" s="11">
+        <f t="shared" si="3"/>
+        <v>17.857142857142875</v>
+      </c>
+      <c r="S9" s="11">
+        <f t="shared" si="3"/>
+        <v>14.285714285714304</v>
+      </c>
+      <c r="T9" s="11">
+        <f t="shared" si="3"/>
+        <v>10.714285714285733</v>
+      </c>
+      <c r="U9" s="11">
+        <f t="shared" si="3"/>
+        <v>7.1428571428571619</v>
+      </c>
+      <c r="V9" s="11">
+        <f t="shared" si="3"/>
+        <v>3.5714285714285903</v>
+      </c>
+      <c r="W9" s="12">
+        <f t="shared" si="3"/>
+        <v>1.865174681370263E-14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4">
+        <v>42794</v>
+      </c>
+      <c r="D1" s="4">
+        <v>42795</v>
+      </c>
+      <c r="E1" s="4">
+        <v>42796</v>
+      </c>
+      <c r="F1" s="4">
+        <v>42797</v>
+      </c>
+      <c r="G1" s="4">
+        <v>42798</v>
+      </c>
+      <c r="H1" s="4">
+        <v>42799</v>
+      </c>
+      <c r="I1" s="4">
+        <v>42800</v>
+      </c>
+      <c r="J1" s="4">
+        <v>42801</v>
+      </c>
+      <c r="K1" s="4">
+        <v>42802</v>
+      </c>
+      <c r="L1" s="4">
+        <v>42803</v>
+      </c>
+      <c r="M1" s="4">
+        <v>42804</v>
+      </c>
+      <c r="N1" s="4">
+        <v>42805</v>
+      </c>
+      <c r="O1" s="4">
+        <v>42806</v>
+      </c>
+      <c r="P1" s="4">
+        <v>42807</v>
+      </c>
+      <c r="Q1" s="4">
+        <v>42808</v>
+      </c>
+      <c r="R1" s="4">
+        <v>42809</v>
+      </c>
+      <c r="S1" s="4">
+        <v>42810</v>
+      </c>
+      <c r="T1" s="4">
+        <v>42811</v>
+      </c>
+      <c r="U1" s="4">
+        <v>42812</v>
+      </c>
+      <c r="V1" s="4">
+        <v>42813</v>
+      </c>
+      <c r="W1" s="4">
+        <v>42814</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="16"/>
       <c r="C2" s="22"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
-      <c r="G2" s="23">
-        <v>1</v>
-      </c>
+      <c r="G2" s="23"/>
       <c r="H2" s="23"/>
-      <c r="I2" s="36">
-        <v>0.5</v>
-      </c>
+      <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
       <c r="L2" s="23"/>
-      <c r="M2" s="23">
-        <v>1</v>
-      </c>
+      <c r="M2" s="23"/>
       <c r="N2" s="23"/>
       <c r="O2" s="23"/>
       <c r="P2" s="23"/>
@@ -5544,9 +6144,7 @@
       <c r="B4" s="16"/>
       <c r="C4" s="25"/>
       <c r="D4" s="26"/>
-      <c r="E4" s="26">
-        <v>1</v>
-      </c>
+      <c r="E4" s="26"/>
       <c r="F4" s="26"/>
       <c r="G4" s="26"/>
       <c r="H4" s="26"/>
@@ -5598,568 +6196,6 @@
         <v>10</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="37">
-        <f>SUM(C2:C5)</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="37">
-        <f t="shared" ref="D6:W6" si="0">SUM(D2:D5)</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="37">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F6" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="37">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H6" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I6" s="37">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="J6" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L6" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M6" s="37">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="N6" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O6" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P6" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R6" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S6" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T6" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U6" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V6" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W6" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="35">
-        <v>75</v>
-      </c>
-      <c r="C7" s="7">
-        <f>B7-C6</f>
-        <v>75</v>
-      </c>
-      <c r="D7" s="7">
-        <f t="shared" ref="D7:W7" si="1">C7-D6</f>
-        <v>75</v>
-      </c>
-      <c r="E7" s="7">
-        <f t="shared" si="1"/>
-        <v>74</v>
-      </c>
-      <c r="F7" s="7">
-        <f t="shared" si="1"/>
-        <v>74</v>
-      </c>
-      <c r="G7" s="7">
-        <f t="shared" si="1"/>
-        <v>73</v>
-      </c>
-      <c r="H7" s="7">
-        <f t="shared" si="1"/>
-        <v>73</v>
-      </c>
-      <c r="I7" s="7">
-        <f t="shared" si="1"/>
-        <v>72.5</v>
-      </c>
-      <c r="J7" s="7">
-        <f t="shared" si="1"/>
-        <v>72.5</v>
-      </c>
-      <c r="K7" s="7">
-        <f t="shared" si="1"/>
-        <v>72.5</v>
-      </c>
-      <c r="L7" s="7">
-        <f t="shared" si="1"/>
-        <v>72.5</v>
-      </c>
-      <c r="M7" s="7">
-        <f t="shared" si="1"/>
-        <v>71.5</v>
-      </c>
-      <c r="N7" s="7">
-        <f t="shared" si="1"/>
-        <v>71.5</v>
-      </c>
-      <c r="O7" s="7">
-        <f t="shared" si="1"/>
-        <v>71.5</v>
-      </c>
-      <c r="P7" s="7">
-        <f t="shared" si="1"/>
-        <v>71.5</v>
-      </c>
-      <c r="Q7" s="7">
-        <f t="shared" si="1"/>
-        <v>71.5</v>
-      </c>
-      <c r="R7" s="7">
-        <f t="shared" si="1"/>
-        <v>71.5</v>
-      </c>
-      <c r="S7" s="7">
-        <f t="shared" si="1"/>
-        <v>71.5</v>
-      </c>
-      <c r="T7" s="7">
-        <f t="shared" si="1"/>
-        <v>71.5</v>
-      </c>
-      <c r="U7" s="7">
-        <f t="shared" si="1"/>
-        <v>71.5</v>
-      </c>
-      <c r="V7" s="7">
-        <f t="shared" si="1"/>
-        <v>71.5</v>
-      </c>
-      <c r="W7" s="2">
-        <f t="shared" si="1"/>
-        <v>71.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="8">
-        <f t="shared" ref="C8:W8" si="2">$B$7/COUNTA($C$1:$W$1)</f>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="D8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="E8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="F8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="G8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="H8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="I8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="J8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="K8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="L8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="M8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="N8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="O8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="P8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="Q8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="R8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="S8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="T8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="U8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="V8" s="8">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="W8" s="9">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11">
-        <f>$B$7-C8</f>
-        <v>71.428571428571431</v>
-      </c>
-      <c r="D9" s="11">
-        <f>C9-D8</f>
-        <v>67.857142857142861</v>
-      </c>
-      <c r="E9" s="11">
-        <f t="shared" ref="E9:W9" si="3">D9-E8</f>
-        <v>64.285714285714292</v>
-      </c>
-      <c r="F9" s="11">
-        <f t="shared" si="3"/>
-        <v>60.714285714285722</v>
-      </c>
-      <c r="G9" s="11">
-        <f t="shared" si="3"/>
-        <v>57.142857142857153</v>
-      </c>
-      <c r="H9" s="11">
-        <f t="shared" si="3"/>
-        <v>53.571428571428584</v>
-      </c>
-      <c r="I9" s="11">
-        <f t="shared" si="3"/>
-        <v>50.000000000000014</v>
-      </c>
-      <c r="J9" s="11">
-        <f t="shared" si="3"/>
-        <v>46.428571428571445</v>
-      </c>
-      <c r="K9" s="11">
-        <f t="shared" si="3"/>
-        <v>42.857142857142875</v>
-      </c>
-      <c r="L9" s="11">
-        <f t="shared" si="3"/>
-        <v>39.285714285714306</v>
-      </c>
-      <c r="M9" s="11">
-        <f t="shared" si="3"/>
-        <v>35.714285714285737</v>
-      </c>
-      <c r="N9" s="11">
-        <f t="shared" si="3"/>
-        <v>32.142857142857167</v>
-      </c>
-      <c r="O9" s="11">
-        <f t="shared" si="3"/>
-        <v>28.571428571428594</v>
-      </c>
-      <c r="P9" s="11">
-        <f t="shared" si="3"/>
-        <v>25.000000000000021</v>
-      </c>
-      <c r="Q9" s="11">
-        <f t="shared" si="3"/>
-        <v>21.428571428571448</v>
-      </c>
-      <c r="R9" s="11">
-        <f t="shared" si="3"/>
-        <v>17.857142857142875</v>
-      </c>
-      <c r="S9" s="11">
-        <f t="shared" si="3"/>
-        <v>14.285714285714304</v>
-      </c>
-      <c r="T9" s="11">
-        <f t="shared" si="3"/>
-        <v>10.714285714285733</v>
-      </c>
-      <c r="U9" s="11">
-        <f t="shared" si="3"/>
-        <v>7.1428571428571619</v>
-      </c>
-      <c r="V9" s="11">
-        <f t="shared" si="3"/>
-        <v>3.5714285714285903</v>
-      </c>
-      <c r="W9" s="12">
-        <f t="shared" si="3"/>
-        <v>1.865174681370263E-14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="4">
-        <v>42794</v>
-      </c>
-      <c r="D1" s="4">
-        <v>42795</v>
-      </c>
-      <c r="E1" s="4">
-        <v>42796</v>
-      </c>
-      <c r="F1" s="4">
-        <v>42797</v>
-      </c>
-      <c r="G1" s="4">
-        <v>42798</v>
-      </c>
-      <c r="H1" s="4">
-        <v>42799</v>
-      </c>
-      <c r="I1" s="4">
-        <v>42800</v>
-      </c>
-      <c r="J1" s="4">
-        <v>42801</v>
-      </c>
-      <c r="K1" s="4">
-        <v>42802</v>
-      </c>
-      <c r="L1" s="4">
-        <v>42803</v>
-      </c>
-      <c r="M1" s="4">
-        <v>42804</v>
-      </c>
-      <c r="N1" s="4">
-        <v>42805</v>
-      </c>
-      <c r="O1" s="4">
-        <v>42806</v>
-      </c>
-      <c r="P1" s="4">
-        <v>42807</v>
-      </c>
-      <c r="Q1" s="4">
-        <v>42808</v>
-      </c>
-      <c r="R1" s="4">
-        <v>42809</v>
-      </c>
-      <c r="S1" s="4">
-        <v>42810</v>
-      </c>
-      <c r="T1" s="4">
-        <v>42811</v>
-      </c>
-      <c r="U1" s="4">
-        <v>42812</v>
-      </c>
-      <c r="V1" s="4">
-        <v>42813</v>
-      </c>
-      <c r="W1" s="4">
-        <v>42814</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="24"/>
-    </row>
-    <row r="3" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="26"/>
-      <c r="U3" s="26"/>
-      <c r="V3" s="26"/>
-      <c r="W3" s="27"/>
-    </row>
-    <row r="4" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="26"/>
-      <c r="V4" s="26"/>
-      <c r="W4" s="27"/>
-    </row>
-    <row r="5" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="30"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="21"/>
       <c r="C6" s="19">
         <f>SUM(C2:C5)</f>
         <v>0</v>
@@ -6531,7 +6567,7 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="34"/>
     <col min="2" max="2" width="16.85546875" style="33" bestFit="1" customWidth="1"/>
@@ -6552,7 +6588,7 @@
       </c>
       <c r="B2" s="33">
         <f>Sprint_One!B7-Sprint_One!W7</f>
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -6588,7 +6624,7 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Updated burndown chart to take the 2 weeks sprint (S2) into account.
</commit_message>
<xml_diff>
--- a/Documentation/Burndown_Chart.xlsx
+++ b/Documentation/Burndown_Chart.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Southampton\solent\Software Systems Development\Scrum\Github\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11310" tabRatio="587"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11310" tabRatio="587" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint_One" sheetId="4" r:id="rId1"/>
@@ -461,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -522,25 +522,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -595,6 +586,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -679,7 +673,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -953,7 +947,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -990,7 +984,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="400622888"/>
@@ -1077,7 +1071,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1109,7 +1103,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="400622560"/>
@@ -1151,7 +1145,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1181,7 +1175,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1257,7 +1251,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1287,72 +1281,51 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sprint_Two!$C$7:$W$7</c:f>
+              <c:f>Sprint_Two!$C$7:$P$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
+                <c:ptCount val="14"/>
+                <c:pt idx="0" formatCode="#,##0\ _€">
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1384,72 +1357,51 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sprint_Two!$C$9:$W$9</c:f>
+              <c:f>Sprint_Two!$C$9:$P$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>23.214285714285715</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>21.428571428571431</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>19.642857142857146</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>17.857142857142861</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>16.071428571428577</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>14.28571428571429</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>12.500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>10.714285714285717</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>8.9285714285714306</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>7.142857142857145</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>5.3571428571428594</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>3.5714285714285738</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1.785714285714288</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>2.2204460492503131E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1531,7 +1483,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1568,7 +1520,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="400622888"/>
@@ -1655,11 +1607,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0\ _€" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1687,7 +1639,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="400622560"/>
@@ -1729,7 +1681,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1759,7 +1711,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1835,7 +1787,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1972,7 +1924,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2010,7 +1962,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="362434424"/>
@@ -2092,7 +2044,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2124,7 +2076,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="362434096"/>
@@ -2165,7 +2117,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2241,7 +2193,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2515,7 +2467,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2552,7 +2504,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="400622888"/>
@@ -2639,7 +2591,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2671,7 +2623,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="400622560"/>
@@ -2713,7 +2665,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2743,7 +2695,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4995,7 +4947,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -5025,14 +4983,20 @@
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -5069,7 +5033,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5104,7 +5074,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvPr id="3" name="Diagramm 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5421,7 +5397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
@@ -5506,209 +5482,209 @@
         <v>6</v>
       </c>
       <c r="B2" s="16"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36">
+      <c r="C2" s="36"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33">
         <v>1</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36">
+      <c r="H2" s="33"/>
+      <c r="I2" s="33">
         <v>0.5</v>
       </c>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36">
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33">
         <v>1</v>
       </c>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
-      <c r="V2" s="36"/>
-      <c r="W2" s="40"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="37"/>
     </row>
     <row r="3" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="16"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42">
+      <c r="C3" s="38"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39">
         <v>0.5</v>
       </c>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42">
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39">
         <v>1.5</v>
       </c>
-      <c r="U3" s="42"/>
-      <c r="V3" s="42"/>
-      <c r="W3" s="43"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="40"/>
     </row>
     <row r="4" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="16"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42">
+      <c r="C4" s="38"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39">
         <v>1</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="42">
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39">
         <v>1</v>
       </c>
-      <c r="S4" s="42"/>
-      <c r="T4" s="42"/>
-      <c r="U4" s="42"/>
-      <c r="V4" s="42"/>
-      <c r="W4" s="43"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="39"/>
+      <c r="V4" s="39"/>
+      <c r="W4" s="40"/>
     </row>
     <row r="5" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="16"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="46"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="42"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="42"/>
+      <c r="V5" s="42"/>
+      <c r="W5" s="43"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="37">
+      <c r="C6" s="34">
         <f>SUM(C2:C5)</f>
         <v>0</v>
       </c>
-      <c r="D6" s="37">
+      <c r="D6" s="34">
         <f t="shared" ref="D6:W6" si="0">SUM(D2:D5)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="37">
+      <c r="E6" s="34">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F6" s="37">
+      <c r="F6" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6" s="37">
+      <c r="G6" s="34">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H6" s="37">
+      <c r="H6" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="37">
+      <c r="I6" s="34">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="J6" s="37">
+      <c r="J6" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K6" s="37">
+      <c r="K6" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L6" s="37">
+      <c r="L6" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M6" s="37">
+      <c r="M6" s="34">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="N6" s="37">
+      <c r="N6" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O6" s="37">
+      <c r="O6" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P6" s="37">
+      <c r="P6" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q6" s="37">
+      <c r="Q6" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R6" s="37">
+      <c r="R6" s="34">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="S6" s="37">
+      <c r="S6" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T6" s="37">
+      <c r="T6" s="34">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="U6" s="37">
+      <c r="U6" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V6" s="37">
+      <c r="V6" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W6" s="38">
+      <c r="W6" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5717,7 +5693,7 @@
       <c r="A7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="35">
+      <c r="B7" s="32">
         <v>75</v>
       </c>
       <c r="C7" s="7">
@@ -5995,10 +5971,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6006,7 +5982,7 @@
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -6014,188 +5990,139 @@
         <v>5</v>
       </c>
       <c r="C1" s="4">
-        <v>42794</v>
+        <v>42801</v>
       </c>
       <c r="D1" s="4">
-        <v>42795</v>
+        <v>42802</v>
       </c>
       <c r="E1" s="4">
-        <v>42796</v>
+        <v>42803</v>
       </c>
       <c r="F1" s="4">
-        <v>42797</v>
+        <v>42804</v>
       </c>
       <c r="G1" s="4">
-        <v>42798</v>
+        <v>42805</v>
       </c>
       <c r="H1" s="4">
-        <v>42799</v>
+        <v>42806</v>
       </c>
       <c r="I1" s="4">
-        <v>42800</v>
+        <v>42807</v>
       </c>
       <c r="J1" s="4">
-        <v>42801</v>
+        <v>42808</v>
       </c>
       <c r="K1" s="4">
-        <v>42802</v>
+        <v>42809</v>
       </c>
       <c r="L1" s="4">
-        <v>42803</v>
+        <v>42810</v>
       </c>
       <c r="M1" s="4">
-        <v>42804</v>
+        <v>42811</v>
       </c>
       <c r="N1" s="4">
-        <v>42805</v>
+        <v>42812</v>
       </c>
       <c r="O1" s="4">
-        <v>42806</v>
+        <v>42813</v>
       </c>
       <c r="P1" s="4">
-        <v>42807</v>
-      </c>
-      <c r="Q1" s="4">
-        <v>42808</v>
-      </c>
-      <c r="R1" s="4">
-        <v>42809</v>
-      </c>
-      <c r="S1" s="4">
-        <v>42810</v>
-      </c>
-      <c r="T1" s="4">
-        <v>42811</v>
-      </c>
-      <c r="U1" s="4">
-        <v>42812</v>
-      </c>
-      <c r="V1" s="4">
-        <v>42813</v>
-      </c>
-      <c r="W1" s="4">
         <v>42814</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
       <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="24"/>
     </row>
-    <row r="3" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="16"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="26"/>
-      <c r="U3" s="26"/>
-      <c r="V3" s="26"/>
-      <c r="W3" s="27"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="25"/>
     </row>
-    <row r="4" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="16"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="26"/>
-      <c r="V4" s="26"/>
-      <c r="W4" s="27"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="25"/>
     </row>
-    <row r="5" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="16"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="30"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="27"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="21"/>
       <c r="C6" s="19">
-        <f>SUM(C2:C5)</f>
+        <f t="shared" ref="C6:P6" si="0">SUM(C2:C5)</f>
         <v>0</v>
       </c>
       <c r="D6" s="19">
-        <f t="shared" ref="D6:W6" si="0">SUM(D2:D5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E6" s="19">
@@ -6242,307 +6169,197 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P6" s="19">
+      <c r="P6" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q6" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R6" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S6" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T6" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U6" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V6" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W6" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="7">
+      <c r="B7" s="32">
+        <v>25</v>
+      </c>
+      <c r="C7" s="44">
         <f>B7-C6</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D7" s="7">
-        <f t="shared" ref="D7:W7" si="1">C7-D6</f>
-        <v>0</v>
+        <f t="shared" ref="D7:P7" si="1">C7-D6</f>
+        <v>25</v>
       </c>
       <c r="E7" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G7" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H7" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I7" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="K7" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="L7" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M7" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="N7" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="O7" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="7">
+        <v>25</v>
+      </c>
+      <c r="P7" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S7" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T7" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="U7" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V7" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="W7" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="8">
-        <f t="shared" ref="C8:W8" si="2">$B$7/COUNTA($C$1:$W$1)</f>
-        <v>0</v>
+        <f>$B$7/COUNTA($C$1:$P$1)</f>
+        <v>1.7857142857142858</v>
       </c>
       <c r="D8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>$B$7/COUNTA($C$1:$P$1)</f>
+        <v>1.7857142857142858</v>
       </c>
       <c r="E8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>$B$7/COUNTA($C$1:$P$1)</f>
+        <v>1.7857142857142858</v>
       </c>
       <c r="F8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>$B$7/COUNTA($C$1:$P$1)</f>
+        <v>1.7857142857142858</v>
       </c>
       <c r="G8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>$B$7/COUNTA($C$1:$P$1)</f>
+        <v>1.7857142857142858</v>
       </c>
       <c r="H8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>$B$7/COUNTA($C$1:$P$1)</f>
+        <v>1.7857142857142858</v>
       </c>
       <c r="I8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>$B$7/COUNTA($C$1:$P$1)</f>
+        <v>1.7857142857142858</v>
       </c>
       <c r="J8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>$B$7/COUNTA($C$1:$P$1)</f>
+        <v>1.7857142857142858</v>
       </c>
       <c r="K8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>$B$7/COUNTA($C$1:$P$1)</f>
+        <v>1.7857142857142858</v>
       </c>
       <c r="L8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>$B$7/COUNTA($C$1:$P$1)</f>
+        <v>1.7857142857142858</v>
       </c>
       <c r="M8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>$B$7/COUNTA($C$1:$P$1)</f>
+        <v>1.7857142857142858</v>
       </c>
       <c r="N8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>$B$7/COUNTA($C$1:$P$1)</f>
+        <v>1.7857142857142858</v>
       </c>
       <c r="O8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="S8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="V8" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="W8" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>$B$7/COUNTA($C$1:$P$1)</f>
+        <v>1.7857142857142858</v>
+      </c>
+      <c r="P8" s="9">
+        <f>$B$7/COUNTA($C$1:$P$1)</f>
+        <v>1.7857142857142858</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="11">
-        <f>$B$7-C8</f>
-        <v>0</v>
+        <f>B7-C8</f>
+        <v>23.214285714285715</v>
       </c>
       <c r="D9" s="11">
-        <f>C9-D8</f>
-        <v>0</v>
+        <f t="shared" ref="D9:P9" si="2">C9-D8</f>
+        <v>21.428571428571431</v>
       </c>
       <c r="E9" s="11">
-        <f t="shared" ref="E9:W9" si="3">D9-E8</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>19.642857142857146</v>
       </c>
       <c r="F9" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>17.857142857142861</v>
       </c>
       <c r="G9" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>16.071428571428577</v>
       </c>
       <c r="H9" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>14.28571428571429</v>
       </c>
       <c r="I9" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>12.500000000000004</v>
       </c>
       <c r="J9" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>10.714285714285717</v>
       </c>
       <c r="K9" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8.9285714285714306</v>
       </c>
       <c r="L9" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>7.142857142857145</v>
       </c>
       <c r="M9" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>5.3571428571428594</v>
       </c>
       <c r="N9" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>3.5714285714285738</v>
       </c>
       <c r="O9" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R9" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S9" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="T9" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U9" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="V9" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W9" s="12">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1.785714285714288</v>
+      </c>
+      <c r="P9" s="12">
+        <f t="shared" si="2"/>
+        <v>2.2204460492503131E-15</v>
       </c>
     </row>
   </sheetData>
@@ -6563,44 +6380,44 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="34"/>
-    <col min="2" max="2" width="16.85546875" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="33"/>
+    <col min="1" max="1" width="11.42578125" style="31"/>
+    <col min="2" max="2" width="16.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="29" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="30">
         <f>Sprint_One!B7-Sprint_One!W7</f>
         <v>6.5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="33">
-        <f>Sprint_Two!B7-Sprint_Two!W7</f>
+      <c r="B3" s="30">
+        <f>Sprint_Two!B7-Sprint_Two!P7</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="31" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="31" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Database setup and connection done
</commit_message>
<xml_diff>
--- a/Documentation/Burndown_Chart.xlsx
+++ b/Documentation/Burndown_Chart.xlsx
@@ -66,7 +66,7 @@
     <author>Konstantin</author>
   </authors>
   <commentList>
-    <comment ref="B7" authorId="0" shapeId="0">
+    <comment ref="B8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>four</t>
+  </si>
+  <si>
+    <t>Konstantin Schaper</t>
   </si>
 </sst>
 </file>
@@ -261,7 +264,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -457,11 +460,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -589,6 +618,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1281,10 +1316,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sprint_Two!$C$7:$P$7</c:f>
+              <c:f>Sprint_Two!$C$8:$W$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0" formatCode="#,##0\ _€">
                   <c:v>25</c:v>
                 </c:pt>
@@ -1326,6 +1361,27 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1357,51 +1413,72 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sprint_Two!$C$9:$P$9</c:f>
+              <c:f>Sprint_Two!$C$10:$W$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>23.214285714285715</c:v>
+                  <c:v>23.80952380952381</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>22.61904761904762</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>21.428571428571431</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>19.642857142857146</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>20.238095238095241</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.047619047619051</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>17.857142857142861</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.071428571428577</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>14.28571428571429</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.500000000000004</c:v>
+                  <c:v>16.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.714285714285717</c:v>
+                  <c:v>15.476190476190482</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.9285714285714306</c:v>
+                  <c:v>14.285714285714292</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.142857142857145</c:v>
+                  <c:v>13.095238095238102</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.3571428571428594</c:v>
+                  <c:v>11.904761904761912</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.5714285714285738</c:v>
+                  <c:v>10.714285714285722</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.785714285714288</c:v>
+                  <c:v>9.5238095238095326</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.2204460492503131E-15</c:v>
+                  <c:v>8.3333333333333428</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.1428571428571521</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.9523809523809614</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.7619047619047707</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.5714285714285801</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.3809523809523894</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.1904761904761989</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.4376949871511897E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4979,13 +5056,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>761999</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5971,10 +6048,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5982,7 +6059,7 @@
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -6031,8 +6108,29 @@
       <c r="P1" s="4">
         <v>42814</v>
       </c>
+      <c r="Q1" s="4">
+        <v>42815</v>
+      </c>
+      <c r="R1" s="4">
+        <v>42816</v>
+      </c>
+      <c r="S1" s="4">
+        <v>42817</v>
+      </c>
+      <c r="T1" s="4">
+        <v>42818</v>
+      </c>
+      <c r="U1" s="4">
+        <v>42819</v>
+      </c>
+      <c r="V1" s="4">
+        <v>42820</v>
+      </c>
+      <c r="W1" s="4">
+        <v>42821</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>6</v>
       </c>
@@ -6051,8 +6149,15 @@
       <c r="N2" s="22"/>
       <c r="O2" s="22"/>
       <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
     </row>
-    <row r="3" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>7</v>
       </c>
@@ -6071,8 +6176,15 @@
       <c r="N3" s="24"/>
       <c r="O3" s="24"/>
       <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="25"/>
+      <c r="W3" s="25"/>
     </row>
-    <row r="4" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>8</v>
       </c>
@@ -6091,275 +6203,430 @@
       <c r="N4" s="24"/>
       <c r="O4" s="24"/>
       <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
     </row>
-    <row r="5" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+      <c r="V5" s="46">
+        <v>7</v>
+      </c>
+      <c r="W5" s="46"/>
+    </row>
+    <row r="6" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="27"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="19">
-        <f t="shared" ref="C6:P6" si="0">SUM(C2:C5)</f>
+      <c r="B7" s="21"/>
+      <c r="C7" s="19">
+        <f>SUM(C2:C6)</f>
         <v>0</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D7" s="19">
+        <f t="shared" ref="D7:P7" si="0">SUM(D2:D6)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E6" s="19">
+      <c r="F7" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F6" s="19">
+      <c r="G7" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6" s="19">
+      <c r="H7" s="19">
+        <f>SUM(H2:H6)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="19">
+      <c r="J7" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="19">
+      <c r="K7" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J6" s="19">
+      <c r="L7" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K6" s="19">
+      <c r="M7" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L6" s="19">
+      <c r="N7" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M6" s="19">
+      <c r="O7" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N6" s="19">
+      <c r="P7" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O6" s="19">
-        <f t="shared" si="0"/>
+      <c r="Q7" s="20">
+        <f t="shared" ref="Q7:V7" si="1">SUM(Q2:Q6)</f>
         <v>0</v>
       </c>
-      <c r="P6" s="20">
-        <f t="shared" si="0"/>
+      <c r="R7" s="20">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="S7" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T7" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U7" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V7" s="20">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="W7" s="20">
+        <f t="shared" ref="W7" si="2">SUM(W2:W6)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B8" s="32">
         <v>25</v>
       </c>
-      <c r="C7" s="44">
-        <f>B7-C6</f>
+      <c r="C8" s="44">
+        <f>B8-C7</f>
         <v>25</v>
       </c>
-      <c r="D7" s="7">
-        <f t="shared" ref="D7:P7" si="1">C7-D6</f>
+      <c r="D8" s="7">
+        <f t="shared" ref="D8:P8" si="3">C8-D7</f>
         <v>25</v>
       </c>
-      <c r="E7" s="7">
-        <f t="shared" si="1"/>
+      <c r="E8" s="7">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="F7" s="7">
-        <f t="shared" si="1"/>
+      <c r="F8" s="7">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="G7" s="7">
-        <f t="shared" si="1"/>
+      <c r="G8" s="7">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="H7" s="7">
-        <f t="shared" si="1"/>
+      <c r="H8" s="7">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="I7" s="7">
-        <f t="shared" si="1"/>
+      <c r="I8" s="7">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="J7" s="7">
-        <f t="shared" si="1"/>
+      <c r="J8" s="7">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="K7" s="7">
-        <f t="shared" si="1"/>
+      <c r="K8" s="7">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="L7" s="7">
-        <f t="shared" si="1"/>
+      <c r="L8" s="7">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="M7" s="7">
-        <f t="shared" si="1"/>
+      <c r="M8" s="7">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="N7" s="7">
-        <f t="shared" si="1"/>
+      <c r="N8" s="7">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="O7" s="7">
-        <f t="shared" si="1"/>
+      <c r="O8" s="7">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="P7" s="2">
-        <f t="shared" si="1"/>
+      <c r="P8" s="2">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
+      <c r="Q8" s="2">
+        <f t="shared" ref="Q8" si="4">P8-Q7</f>
+        <v>25</v>
+      </c>
+      <c r="R8" s="2">
+        <f t="shared" ref="R8" si="5">Q8-R7</f>
+        <v>25</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" ref="S8" si="6">R8-S7</f>
+        <v>25</v>
+      </c>
+      <c r="T8" s="2">
+        <f t="shared" ref="T8" si="7">S8-T7</f>
+        <v>25</v>
+      </c>
+      <c r="U8" s="2">
+        <f t="shared" ref="U8:W8" si="8">T8-U7</f>
+        <v>25</v>
+      </c>
+      <c r="V8" s="2">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+      <c r="W8" s="2">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="8">
-        <f>$B$7/COUNTA($C$1:$P$1)</f>
-        <v>1.7857142857142858</v>
-      </c>
-      <c r="D8" s="8">
-        <f>$B$7/COUNTA($C$1:$P$1)</f>
-        <v>1.7857142857142858</v>
-      </c>
-      <c r="E8" s="8">
-        <f>$B$7/COUNTA($C$1:$P$1)</f>
-        <v>1.7857142857142858</v>
-      </c>
-      <c r="F8" s="8">
-        <f>$B$7/COUNTA($C$1:$P$1)</f>
-        <v>1.7857142857142858</v>
-      </c>
-      <c r="G8" s="8">
-        <f>$B$7/COUNTA($C$1:$P$1)</f>
-        <v>1.7857142857142858</v>
-      </c>
-      <c r="H8" s="8">
-        <f>$B$7/COUNTA($C$1:$P$1)</f>
-        <v>1.7857142857142858</v>
-      </c>
-      <c r="I8" s="8">
-        <f>$B$7/COUNTA($C$1:$P$1)</f>
-        <v>1.7857142857142858</v>
-      </c>
-      <c r="J8" s="8">
-        <f>$B$7/COUNTA($C$1:$P$1)</f>
-        <v>1.7857142857142858</v>
-      </c>
-      <c r="K8" s="8">
-        <f>$B$7/COUNTA($C$1:$P$1)</f>
-        <v>1.7857142857142858</v>
-      </c>
-      <c r="L8" s="8">
-        <f>$B$7/COUNTA($C$1:$P$1)</f>
-        <v>1.7857142857142858</v>
-      </c>
-      <c r="M8" s="8">
-        <f>$B$7/COUNTA($C$1:$P$1)</f>
-        <v>1.7857142857142858</v>
-      </c>
-      <c r="N8" s="8">
-        <f>$B$7/COUNTA($C$1:$P$1)</f>
-        <v>1.7857142857142858</v>
-      </c>
-      <c r="O8" s="8">
-        <f>$B$7/COUNTA($C$1:$P$1)</f>
-        <v>1.7857142857142858</v>
-      </c>
-      <c r="P8" s="9">
-        <f>$B$7/COUNTA($C$1:$P$1)</f>
-        <v>1.7857142857142858</v>
+      <c r="B9" s="2"/>
+      <c r="C9" s="8">
+        <f>$B$8/COUNTA($C$1:$W$1)</f>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="D9" s="8">
+        <f>$C$9</f>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="E9" s="8">
+        <f t="shared" ref="E9:W9" si="9">$C$9</f>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="F9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="G9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="H9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="I9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="J9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="K9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="L9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="M9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="N9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="O9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="P9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="Q9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="R9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="S9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="T9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="U9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="V9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="W9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1904761904761905</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11">
-        <f>B7-C8</f>
-        <v>23.214285714285715</v>
-      </c>
-      <c r="D9" s="11">
-        <f t="shared" ref="D9:P9" si="2">C9-D8</f>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11">
+        <f>B8-C9</f>
+        <v>23.80952380952381</v>
+      </c>
+      <c r="D10" s="11">
+        <f t="shared" ref="D10:P10" si="10">C10-D9</f>
+        <v>22.61904761904762</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" si="10"/>
         <v>21.428571428571431</v>
       </c>
-      <c r="E9" s="11">
-        <f t="shared" si="2"/>
-        <v>19.642857142857146</v>
-      </c>
-      <c r="F9" s="11">
-        <f t="shared" si="2"/>
+      <c r="F10" s="11">
+        <f t="shared" si="10"/>
+        <v>20.238095238095241</v>
+      </c>
+      <c r="G10" s="11">
+        <f t="shared" si="10"/>
+        <v>19.047619047619051</v>
+      </c>
+      <c r="H10" s="11">
+        <f t="shared" si="10"/>
         <v>17.857142857142861</v>
       </c>
-      <c r="G9" s="11">
-        <f t="shared" si="2"/>
-        <v>16.071428571428577</v>
-      </c>
-      <c r="H9" s="11">
-        <f t="shared" si="2"/>
-        <v>14.28571428571429</v>
-      </c>
-      <c r="I9" s="11">
-        <f t="shared" si="2"/>
-        <v>12.500000000000004</v>
-      </c>
-      <c r="J9" s="11">
-        <f t="shared" si="2"/>
-        <v>10.714285714285717</v>
-      </c>
-      <c r="K9" s="11">
-        <f t="shared" si="2"/>
-        <v>8.9285714285714306</v>
-      </c>
-      <c r="L9" s="11">
-        <f t="shared" si="2"/>
-        <v>7.142857142857145</v>
-      </c>
-      <c r="M9" s="11">
-        <f t="shared" si="2"/>
-        <v>5.3571428571428594</v>
-      </c>
-      <c r="N9" s="11">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285738</v>
-      </c>
-      <c r="O9" s="11">
-        <f t="shared" si="2"/>
-        <v>1.785714285714288</v>
-      </c>
-      <c r="P9" s="12">
-        <f t="shared" si="2"/>
-        <v>2.2204460492503131E-15</v>
+      <c r="I10" s="11">
+        <f t="shared" si="10"/>
+        <v>16.666666666666671</v>
+      </c>
+      <c r="J10" s="11">
+        <f t="shared" si="10"/>
+        <v>15.476190476190482</v>
+      </c>
+      <c r="K10" s="11">
+        <f t="shared" si="10"/>
+        <v>14.285714285714292</v>
+      </c>
+      <c r="L10" s="11">
+        <f t="shared" si="10"/>
+        <v>13.095238095238102</v>
+      </c>
+      <c r="M10" s="11">
+        <f t="shared" si="10"/>
+        <v>11.904761904761912</v>
+      </c>
+      <c r="N10" s="11">
+        <f t="shared" si="10"/>
+        <v>10.714285714285722</v>
+      </c>
+      <c r="O10" s="11">
+        <f t="shared" si="10"/>
+        <v>9.5238095238095326</v>
+      </c>
+      <c r="P10" s="12">
+        <f t="shared" si="10"/>
+        <v>8.3333333333333428</v>
+      </c>
+      <c r="Q10" s="12">
+        <f t="shared" ref="Q10" si="11">P10-Q9</f>
+        <v>7.1428571428571521</v>
+      </c>
+      <c r="R10" s="12">
+        <f t="shared" ref="R10" si="12">Q10-R9</f>
+        <v>5.9523809523809614</v>
+      </c>
+      <c r="S10" s="12">
+        <f t="shared" ref="S10" si="13">R10-S9</f>
+        <v>4.7619047619047707</v>
+      </c>
+      <c r="T10" s="12">
+        <f t="shared" ref="T10" si="14">S10-T9</f>
+        <v>3.5714285714285801</v>
+      </c>
+      <c r="U10" s="12">
+        <f t="shared" ref="U10:W10" si="15">T10-U9</f>
+        <v>2.3809523809523894</v>
+      </c>
+      <c r="V10" s="12">
+        <f t="shared" si="15"/>
+        <v>1.1904761904761989</v>
+      </c>
+      <c r="W10" s="12">
+        <f t="shared" si="15"/>
+        <v>8.4376949871511897E-15</v>
       </c>
     </row>
   </sheetData>
@@ -6407,7 +6674,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="30">
-        <f>Sprint_Two!B7-Sprint_Two!P7</f>
+        <f>Sprint_Two!B8-Sprint_Two!P8</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Membership Information Display done, Member browsing done, ServiceRegistry unit tests written and successful, Burndown Chart updated
</commit_message>
<xml_diff>
--- a/Documentation/Burndown_Chart.xlsx
+++ b/Documentation/Burndown_Chart.xlsx
@@ -1381,7 +1381,7 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>17</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6050,8 +6050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6238,7 +6238,9 @@
       <c r="V5" s="46">
         <v>8</v>
       </c>
-      <c r="W5" s="46"/>
+      <c r="W5" s="46">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
@@ -6354,7 +6356,7 @@
       </c>
       <c r="W7" s="20">
         <f t="shared" ref="W7" si="2">SUM(W2:W6)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -6446,7 +6448,7 @@
       </c>
       <c r="W8" s="2">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated burndown chart velocity for sprint 2
</commit_message>
<xml_diff>
--- a/Documentation/Burndown_Chart.xlsx
+++ b/Documentation/Burndown_Chart.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Southampton\solent\Software Systems Development\Scrum\Github\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3schak76\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11310" tabRatio="587" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" tabRatio="587" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint_One" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Velocity_Chart" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint_One (Deprecated)" sheetId="1" state="hidden" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0\ _€"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -628,7 +628,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -644,9 +644,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -708,7 +708,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -809,7 +809,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6563-483E-A12C-864B2E4FE692}"/>
             </c:ext>
@@ -906,7 +906,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6563-483E-A12C-864B2E4FE692}"/>
             </c:ext>
@@ -921,11 +921,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="400622560"/>
-        <c:axId val="400622888"/>
+        <c:axId val="493794824"/>
+        <c:axId val="493795216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="400622560"/>
+        <c:axId val="493794824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -982,7 +982,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1019,10 +1019,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400622888"/>
+        <c:crossAx val="493795216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1030,7 +1030,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="400622888"/>
+        <c:axId val="493795216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1106,7 +1106,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1138,10 +1138,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400622560"/>
+        <c:crossAx val="493794824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1180,7 +1180,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1210,7 +1210,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1222,9 +1222,1000 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Burndown-Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Actual</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint_Two!$C$8:$W$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0" formatCode="#,##0\ _€">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8A22-4D2A-B82F-502C025A796D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ideal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint_Two!$C$10:$W$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>23.80952380952381</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.61904761904762</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.428571428571431</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.238095238095241</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.047619047619051</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.857142857142861</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.666666666666671</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.476190476190482</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.285714285714292</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.095238095238102</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.904761904761912</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.714285714285722</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.5238095238095326</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.3333333333333428</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.1428571428571521</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.9523809523809614</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.7619047619047707</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.5714285714285801</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.3809523809523894</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.1904761904761989</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.4376949871511897E-15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8A22-4D2A-B82F-502C025A796D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="495479104"/>
+        <c:axId val="495479496"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="495479104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Days in Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="495479496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="495479496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Remaining</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Effort Hours</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0\ _€" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="495479104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Velocity Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Velocity_Chart!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>one</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>two</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>three</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>four</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Velocity_Chart!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-0ED7-4308-8C5A-9471866D8495}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="495480280"/>
+        <c:axId val="495480672"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="495480280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="495480672"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="495480672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Work Done</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="495480280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1286,7 +2277,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1316,80 +2307,80 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sprint_Two!$C$8:$W$8</c:f>
+              <c:f>'Sprint_One (Deprecated)'!$C$3:$W$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
-                <c:pt idx="0" formatCode="#,##0\ _€">
-                  <c:v>25</c:v>
+                <c:pt idx="0">
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>25</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>25</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>25</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>25</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>25</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>17</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8A22-4D2A-B82F-502C025A796D}"/>
+              <c16:uniqueId val="{00000000-9251-4BA3-ADAD-D0E9A2AE2542}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1413,80 +2404,80 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sprint_Two!$C$10:$W$10</c:f>
+              <c:f>'Sprint_One (Deprecated)'!$C$5:$W$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>23.80952380952381</c:v>
+                  <c:v>73.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.61904761904762</c:v>
+                  <c:v>69.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.428571428571431</c:v>
+                  <c:v>65.999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.238095238095241</c:v>
+                  <c:v>62.333333333333321</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.047619047619051</c:v>
+                  <c:v>58.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.857142857142861</c:v>
+                  <c:v>54.999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.666666666666671</c:v>
+                  <c:v>51.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15.476190476190482</c:v>
+                  <c:v>47.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14.285714285714292</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.095238095238102</c:v>
+                  <c:v>40.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.904761904761912</c:v>
+                  <c:v>36.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10.714285714285722</c:v>
+                  <c:v>33.000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.5238095238095326</c:v>
+                  <c:v>29.333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.3333333333333428</c:v>
+                  <c:v>25.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.1428571428571521</c:v>
+                  <c:v>22.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.9523809523809614</c:v>
+                  <c:v>18.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.7619047619047707</c:v>
+                  <c:v>14.66666666666667</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.5714285714285801</c:v>
+                  <c:v>11.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.3809523809523894</c:v>
+                  <c:v>7.3333333333333375</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.1904761904761989</c:v>
+                  <c:v>3.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8.4376949871511897E-15</c:v>
+                  <c:v>4.4408920985006262E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8A22-4D2A-B82F-502C025A796D}"/>
+              <c16:uniqueId val="{00000001-9251-4BA3-ADAD-D0E9A2AE2542}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1499,11 +2490,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="400622560"/>
-        <c:axId val="400622888"/>
+        <c:axId val="495481456"/>
+        <c:axId val="495481848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="400622560"/>
+        <c:axId val="495481456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1560,7 +2551,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1597,10 +2588,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400622888"/>
+        <c:crossAx val="495481848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1608,7 +2599,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="400622888"/>
+        <c:axId val="495481848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1684,11 +2675,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="#,##0\ _€" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1716,10 +2707,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400622560"/>
+        <c:crossAx val="495481456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1758,7 +2749,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1788,991 +2779,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Velocity Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Velocity_Chart!$A$2:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>one</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>two</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>three</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>four</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Velocity_Chart!$B$2:$B$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-0ED7-4308-8C5A-9471866D8495}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="362434096"/>
-        <c:axId val="362434424"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="362434096"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="362434424"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="362434424"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Work Done</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="362434096"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Burndown-Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Actual</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint_One (Deprecated)'!$C$3:$W$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>74.5</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>74.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9251-4BA3-ADAD-D0E9A2AE2542}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Ideal</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint_One (Deprecated)'!$C$5:$W$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>73.333333333333329</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>69.666666666666657</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>65.999999999999986</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>62.333333333333321</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>58.666666666666657</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>54.999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>51.333333333333329</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>47.666666666666664</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>40.333333333333336</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>36.666666666666671</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>33.000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>29.333333333333339</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>25.666666666666671</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>22.000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>18.333333333333336</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>14.66666666666667</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>11.000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>7.3333333333333375</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.666666666666671</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4.4408920985006262E-15</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9251-4BA3-ADAD-D0E9A2AE2542}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="400622560"/>
-        <c:axId val="400622888"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="400622560"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Days in Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="400622888"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="400622888"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Remaining</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Effort Hours</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="400622560"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5027,7 +5034,7 @@
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5070,7 +5077,7 @@
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5113,7 +5120,7 @@
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5154,7 +5161,7 @@
         <xdr:cNvPr id="3" name="Diagramm 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5478,7 +5485,7 @@
       <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
   </cols>
@@ -6050,11 +6057,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
   </cols>
@@ -6643,11 +6650,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="31"/>
     <col min="2" max="2" width="16.85546875" style="30" bestFit="1" customWidth="1"/>
@@ -6676,8 +6683,8 @@
         <v>16</v>
       </c>
       <c r="B3" s="30">
-        <f>Sprint_Two!B8-Sprint_Two!P8</f>
-        <v>0</v>
+        <f>Sprint_Two!B8-Sprint_Two!W8</f>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -6704,7 +6711,7 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>